<commit_message>
intermediate revision - adding headers so the "TestData.xlsx" can be queried via FILLO SQL
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -6,36 +6,60 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="test123" r:id="rId3" sheetId="1"/>
+    <sheet name="Test Status" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+  <si>
+    <t>Test Method</t>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
   <si>
     <t>testOne</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>testSeven</t>
+  </si>
+  <si>
+    <t>testThree</t>
+  </si>
+  <si>
+    <t>testSix</t>
+  </si>
+  <si>
+    <t>testNine</t>
+  </si>
+  <si>
+    <t>testFour</t>
+  </si>
+  <si>
     <t>true</t>
-  </si>
-  <si>
-    <t>testSeven</t>
-  </si>
-  <si>
-    <t>testThree</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>testSix</t>
-  </si>
-  <si>
-    <t>testNine</t>
-  </si>
-  <si>
-    <t>testFour</t>
   </si>
   <si>
     <t>testEight</t>
@@ -92,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -105,77 +129,103 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
intermediate revision - enabled collection of the data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Test Method</t>
   </si>
@@ -20,22 +20,7 @@
     <t>Run 1</t>
   </si>
   <si>
-    <t>Run 2</t>
-  </si>
-  <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
+    <t>Row 2</t>
   </si>
   <si>
     <t>testOne</t>
@@ -50,6 +35,9 @@
     <t>testThree</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>testSix</t>
   </si>
   <si>
@@ -57,9 +45,6 @@
   </si>
   <si>
     <t>testFour</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>testEight</t>
@@ -116,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -132,100 +117,85 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>